<commit_message>
Revisiting checked to include cat1
</commit_message>
<xml_diff>
--- a/data/feature_analysis_results.xlsx
+++ b/data/feature_analysis_results.xlsx
@@ -8460,10 +8460,10 @@
         </is>
       </c>
       <c r="B62" s="1" t="n">
-        <v>23</v>
+        <v>201</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>91</v>
+        <v>229</v>
       </c>
       <c r="D62" s="1" t="n">
         <v>334</v>
@@ -8472,64 +8472,64 @@
         <v>342</v>
       </c>
       <c r="F62" s="1" t="n">
+        <v>410</v>
+      </c>
+      <c r="G62" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="H62" s="1" t="n">
+        <v>549</v>
+      </c>
+      <c r="I62" s="1" t="n">
+        <v>625</v>
+      </c>
+      <c r="J62" s="1" t="n">
+        <v>678</v>
+      </c>
+      <c r="K62" s="1" t="n">
+        <v>712</v>
+      </c>
+      <c r="L62" s="1" t="n">
+        <v>799</v>
+      </c>
+      <c r="M62" s="1" t="n">
+        <v>871</v>
+      </c>
+      <c r="N62" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="O62" s="1" t="n">
         <v>351</v>
       </c>
-      <c r="G62" s="1" t="n">
+      <c r="P62" s="1" t="n">
         <v>375</v>
       </c>
-      <c r="H62" s="1" t="n">
-        <v>410</v>
-      </c>
-      <c r="I62" s="1" t="n">
-        <v>494</v>
-      </c>
-      <c r="J62" s="1" t="n">
+      <c r="Q62" s="1" t="n">
         <v>541</v>
       </c>
-      <c r="K62" s="1" t="n">
-        <v>549</v>
-      </c>
-      <c r="L62" s="1" t="n">
+      <c r="R62" s="1" t="n">
         <v>565</v>
       </c>
-      <c r="M62" s="1" t="n">
-        <v>625</v>
-      </c>
-      <c r="N62" s="1" t="n">
-        <v>678</v>
-      </c>
-      <c r="O62" s="1" t="n">
-        <v>712</v>
-      </c>
-      <c r="P62" s="1" t="n">
+      <c r="S62" s="1" t="n">
         <v>725</v>
-      </c>
-      <c r="Q62" s="1" t="n">
-        <v>799</v>
-      </c>
-      <c r="R62" s="1" t="n">
-        <v>864</v>
-      </c>
-      <c r="S62" s="1" t="n">
-        <v>871</v>
       </c>
       <c r="T62" s="1" t="n">
         <v>863</v>
       </c>
       <c r="U62" s="1" t="n">
-        <v>201</v>
+        <v>864</v>
       </c>
       <c r="V62" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="W62" s="1" t="n">
         <v>214</v>
-      </c>
-      <c r="W62" s="1" t="n">
-        <v>229</v>
       </c>
       <c r="X62" s="1" t="n">
         <v>408</v>
       </c>
       <c r="Y62" s="1" t="n">
-        <v>471</v>
+        <v>494</v>
       </c>
       <c r="Z62" s="1" t="n">
         <v>526</v>
@@ -8606,32 +8606,32 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="S63" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="T63" t="inlineStr">
@@ -8641,7 +8641,7 @@
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
@@ -8712,132 +8712,132 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>9/17 (52.9%)</t>
+          <t>1/17 (5.9%)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>11/17 (64.7%)</t>
+          <t>5/17 (29.4%)</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>8/17 (47.1%)</t>
+          <t>4/17 (23.5%)</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
           <t>2/17 (11.8%)</t>
         </is>
       </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>11/17 (64.7%)</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>11/17 (64.7%)</t>
-        </is>
-      </c>
       <c r="H65" t="inlineStr">
         <is>
+          <t>4/17 (23.5%)</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>5/17 (29.4%)</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>3/17 (17.6%)</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
           <t>2/17 (11.8%)</t>
         </is>
       </c>
-      <c r="I65" t="inlineStr">
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
         <is>
           <t>2/17 (11.8%)</t>
         </is>
       </c>
-      <c r="J65" t="inlineStr">
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>2/17 (11.8%)</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>6/17 (35.3%)</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
         <is>
           <t>3/17 (17.6%)</t>
         </is>
       </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>14/17 (82.4%)</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>9/17 (52.9%)</t>
-        </is>
-      </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>10/17 (58.8%)</t>
-        </is>
-      </c>
-      <c r="N65" t="inlineStr">
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>3/17 (17.6%)</t>
+        </is>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="T65" t="inlineStr">
         <is>
           <t>7/17 (41.2%)</t>
         </is>
       </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>5/17 (29.4%)</t>
-        </is>
-      </c>
-      <c r="P65" t="inlineStr">
-        <is>
-          <t>9/17 (52.9%)</t>
-        </is>
-      </c>
-      <c r="Q65" t="inlineStr">
+      <c r="U65" t="inlineStr">
         <is>
           <t>2/17 (11.8%)</t>
         </is>
       </c>
-      <c r="R65" t="inlineStr">
-        <is>
-          <t>11/17 (64.7%)</t>
-        </is>
-      </c>
-      <c r="S65" t="inlineStr">
-        <is>
-          <t>6/17 (35.3%)</t>
-        </is>
-      </c>
-      <c r="T65" t="inlineStr">
-        <is>
-          <t>10/17 (58.8%)</t>
-        </is>
-      </c>
-      <c r="U65" t="inlineStr">
+      <c r="V65" t="inlineStr">
+        <is>
+          <t>7/17 (41.2%)</t>
+        </is>
+      </c>
+      <c r="W65" t="inlineStr">
+        <is>
+          <t>4/17 (23.5%)</t>
+        </is>
+      </c>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>7/17 (41.2%)</t>
+        </is>
+      </c>
+      <c r="Y65" t="inlineStr">
         <is>
           <t>0/17 (0.0%)</t>
         </is>
       </c>
-      <c r="V65" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="W65" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="X65" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="Y65" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
       <c r="Z65" t="inlineStr">
         <is>
-          <t>0/17 (0.0%)</t>
+          <t>3/17 (17.6%)</t>
         </is>
       </c>
       <c r="AA65" t="inlineStr">
         <is>
-          <t>0/17 (0.0%)</t>
+          <t>2/17 (11.8%)</t>
         </is>
       </c>
     </row>
@@ -8849,117 +8849,117 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>0.2877</t>
+          <t>0.0006</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>0.9006</t>
+          <t>1.0213</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>0.2478</t>
+          <t>0.2403</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>0.0004</t>
+          <t>0.0002</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>0.7303</t>
+          <t>0.0001</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>0.7887</t>
+          <t>0.3676</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>0.0002</t>
+          <t>0.6593</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>0.0003</t>
+          <t>0.2304</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>0.0022</t>
+          <t>0.2794</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>1.3636</t>
+          <t>0.6123</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>0.4559</t>
+          <t>0.0001</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>0.4446</t>
+          <t>0.1833</t>
         </is>
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>0.2886</t>
+          <t>0.0026</t>
         </is>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>1.2359</t>
+          <t>0.3639</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>0.5820</t>
+          <t>0.0538</t>
         </is>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>0.0002</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
         <is>
-          <t>0.4482</t>
+          <t>0.0133</t>
         </is>
       </c>
       <c r="S66" t="inlineStr">
         <is>
-          <t>0.3658</t>
+          <t>0.0005</t>
         </is>
       </c>
       <c r="T66" t="inlineStr">
         <is>
-          <t>0.4485</t>
+          <t>0.2060</t>
         </is>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0093</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.5332</t>
         </is>
       </c>
       <c r="W66" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.4934</t>
         </is>
       </c>
       <c r="X66" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0624</t>
         </is>
       </c>
       <c r="Y66" t="inlineStr">
@@ -8969,12 +8969,12 @@
       </c>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0909</t>
         </is>
       </c>
       <c r="AA66" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.1435</t>
         </is>
       </c>
     </row>
@@ -8986,132 +8986,132 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>1/32 (3.1%)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>16/32 (50.0%)</t>
+          <t>12/32 (37.5%)</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>3/32 (9.4%)</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>1/32 (3.1%)</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>16/32 (50.0%)</t>
+          <t>1/32 (3.1%)</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>3/32 (9.4%)</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>8/32 (25.0%)</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>4/32 (12.5%)</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>3/32 (9.4%)</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>2/32 (6.2%)</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>1/32 (3.1%)</t>
         </is>
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>3/32 (9.4%)</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>5/32 (15.6%)</t>
         </is>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>14/32 (43.8%)</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>6/32 (18.8%)</t>
         </is>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>2/32 (6.2%)</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>4/32 (12.5%)</t>
         </is>
       </c>
       <c r="S67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>6/32 (18.8%)</t>
         </is>
       </c>
       <c r="T67" t="inlineStr">
         <is>
-          <t>19/32 (59.4%)</t>
+          <t>14/32 (43.8%)</t>
         </is>
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>6/32 (18.8%)</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>8/32 (25.0%)</t>
+          <t>12/32 (37.5%)</t>
         </is>
       </c>
       <c r="W67" t="inlineStr">
         <is>
-          <t>12/32 (37.5%)</t>
+          <t>7/32 (21.9%)</t>
         </is>
       </c>
       <c r="X67" t="inlineStr">
         <is>
-          <t>14/32 (43.8%)</t>
+          <t>11/32 (34.4%)</t>
         </is>
       </c>
       <c r="Y67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>1/32 (3.1%)</t>
         </is>
       </c>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>6/32 (18.8%)</t>
         </is>
       </c>
       <c r="AA67" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>3/32 (9.4%)</t>
         </is>
       </c>
     </row>
@@ -9123,52 +9123,52 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0005</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>0.5326</t>
+          <t>0.2524</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0006</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0001</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>0.2684</t>
+          <t>0.0001</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0656</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.3253</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0007</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0007</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0009</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
@@ -9178,77 +9178,77 @@
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0016</t>
         </is>
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.1118</t>
         </is>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.4086</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.3656</t>
         </is>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0011</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.2257</t>
         </is>
       </c>
       <c r="S68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.2992</t>
         </is>
       </c>
       <c r="T68" t="inlineStr">
         <is>
-          <t>0.5028</t>
+          <t>0.4255</t>
         </is>
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.1261</t>
         </is>
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>0.2834</t>
+          <t>0.2808</t>
         </is>
       </c>
       <c r="W68" t="inlineStr">
         <is>
-          <t>0.1405</t>
+          <t>0.6310</t>
         </is>
       </c>
       <c r="X68" t="inlineStr">
         <is>
-          <t>0.1243</t>
+          <t>0.0713</t>
         </is>
       </c>
       <c r="Y68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0001</t>
         </is>
       </c>
       <c r="Z68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.1514</t>
         </is>
       </c>
       <c r="AA68" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0094</t>
         </is>
       </c>
     </row>
@@ -9260,97 +9260,97 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>8/21 (38.1%)</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
           <t>0/21 (0.0%)</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="F69" t="inlineStr">
         <is>
           <t>0/21 (0.0%)</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>4/21 (19.0%)</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>2/21 (9.5%)</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
         <is>
           <t>0/21 (0.0%)</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>0/21 (0.0%)</t>
+          <t>1/21 (4.8%)</t>
         </is>
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>0/21 (0.0%)</t>
+          <t>2/21 (9.5%)</t>
         </is>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>0/21 (0.0%)</t>
+          <t>7/21 (33.3%)</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>0/21 (0.0%)</t>
+          <t>2/21 (9.5%)</t>
         </is>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>0/21 (0.0%)</t>
+          <t>1/21 (4.8%)</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
         <is>
-          <t>0/21 (0.0%)</t>
+          <t>2/21 (9.5%)</t>
         </is>
       </c>
       <c r="S69" t="inlineStr">
         <is>
-          <t>0/21 (0.0%)</t>
+          <t>2/21 (9.5%)</t>
         </is>
       </c>
       <c r="T69" t="inlineStr">
         <is>
-          <t>0/21 (0.0%)</t>
+          <t>8/21 (38.1%)</t>
         </is>
       </c>
       <c r="U69" t="inlineStr">
@@ -9360,32 +9360,32 @@
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>11/21 (52.4%)</t>
+          <t>8/21 (38.1%)</t>
         </is>
       </c>
       <c r="W69" t="inlineStr">
         <is>
-          <t>13/21 (61.9%)</t>
+          <t>8/21 (38.1%)</t>
         </is>
       </c>
       <c r="X69" t="inlineStr">
         <is>
-          <t>13/21 (61.9%)</t>
+          <t>9/21 (42.9%)</t>
         </is>
       </c>
       <c r="Y69" t="inlineStr">
         <is>
-          <t>9/21 (42.9%)</t>
+          <t>1/21 (4.8%)</t>
         </is>
       </c>
       <c r="Z69" t="inlineStr">
         <is>
-          <t>15/21 (71.4%)</t>
+          <t>6/21 (28.6%)</t>
         </is>
       </c>
       <c r="AA69" t="inlineStr">
         <is>
-          <t>9/21 (42.9%)</t>
+          <t>4/21 (19.0%)</t>
         </is>
       </c>
     </row>
@@ -9397,17 +9397,17 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0007</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.1885</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0052</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -9422,27 +9422,27 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0473</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0745</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.1723</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0063</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.5035</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -9452,77 +9452,77 @@
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.1453</t>
         </is>
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0604</t>
         </is>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0830</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0378</t>
         </is>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0002</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0142</t>
         </is>
       </c>
       <c r="S70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0148</t>
         </is>
       </c>
       <c r="T70" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.3141</t>
         </is>
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>0.0019</t>
+          <t>0.1632</t>
         </is>
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>1.5101</t>
+          <t>0.6811</t>
         </is>
       </c>
       <c r="W70" t="inlineStr">
         <is>
-          <t>1.1856</t>
+          <t>0.5811</t>
         </is>
       </c>
       <c r="X70" t="inlineStr">
         <is>
-          <t>0.4315</t>
+          <t>0.4618</t>
         </is>
       </c>
       <c r="Y70" t="inlineStr">
         <is>
-          <t>0.4448</t>
+          <t>0.0002</t>
         </is>
       </c>
       <c r="Z70" t="inlineStr">
         <is>
-          <t>0.4884</t>
+          <t>0.1842</t>
         </is>
       </c>
       <c r="AA70" t="inlineStr">
         <is>
-          <t>0.2507</t>
+          <t>0.1202</t>
         </is>
       </c>
     </row>
@@ -15951,22 +15951,22 @@
         </is>
       </c>
       <c r="B98" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="C98" s="1" t="n">
         <v>541</v>
       </c>
-      <c r="C98" s="1" t="n">
+      <c r="D98" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="E98" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="F98" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="G98" s="1" t="n">
         <v>549</v>
-      </c>
-      <c r="D98" s="1" t="n">
-        <v>238</v>
-      </c>
-      <c r="E98" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="F98" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="G98" s="1" t="n">
-        <v>211</v>
       </c>
       <c r="H98" s="1" t="n">
         <v>578</v>
@@ -16004,37 +16004,37 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 2</t>
         </is>
       </c>
     </row>
@@ -16059,32 +16059,32 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>3/17 (17.6%)</t>
+          <t>2/17 (11.8%)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>14/17 (82.4%)</t>
+          <t>2/17 (11.8%)</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>0/17 (0.0%)</t>
+          <t>15/17 (88.2%)</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>17/17 (100.0%)</t>
+          <t>1/17 (5.9%)</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>0/17 (0.0%)</t>
+          <t>1/17 (5.9%)</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>0/17 (0.0%)</t>
+          <t>10/17 (58.8%)</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -16116,32 +16116,32 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>0.0022</t>
+          <t>5.1452</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>1.3636</t>
+          <t>0.0015</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>3.5077</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>3.7249</t>
+          <t>0.0006</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0003</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.2309</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -16173,52 +16173,52 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>1/32 (3.1%)</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>14/32 (43.8%)</t>
+          <t>1/32 (3.1%)</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>3/32 (9.4%)</t>
+          <t>28/32 (87.5%)</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>26/32 (81.2%)</t>
+          <t>2/32 (6.2%)</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>2/32 (6.2%)</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>21/32 (65.6%)</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>1/32 (3.1%)</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>2/32 (6.2%)</t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>2/32 (6.2%)</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>0/32 (0.0%)</t>
+          <t>1/32 (3.1%)</t>
         </is>
       </c>
     </row>
@@ -16230,52 +16230,52 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.3389</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>0.1728</t>
+          <t>0.0004</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>3.0723</t>
+          <t>6.4179</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>5.3619</t>
+          <t>0.0009</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0005</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.6389</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0006</t>
         </is>
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0007</t>
         </is>
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0007</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0007</t>
         </is>
       </c>
     </row>
@@ -16292,47 +16292,47 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>12/21 (57.1%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
+          <t>18/21 (85.7%)</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
           <t>0/21 (0.0%)</t>
         </is>
       </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>18/21 (85.7%)</t>
-        </is>
-      </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>3/21 (14.3%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>3/21 (14.3%)</t>
+          <t>9/21 (42.9%)</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>2/21 (9.5%)</t>
+          <t>1/21 (4.8%)</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>2/21 (9.5%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>2/21 (9.5%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>1/21 (4.8%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
     </row>
@@ -16349,47 +16349,47 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>0.0762</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>5.5161</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>6.9495</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>0.0019</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>0.0009</t>
+          <t>0.2830</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>0.0011</t>
+          <t>0.0001</t>
         </is>
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>0.0011</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>0.0011</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>0.0011</t>
+          <t>0.0000</t>
         </is>
       </c>
     </row>
@@ -16407,43 +16407,43 @@
         </is>
       </c>
       <c r="B110" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="C110" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="D110" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="E110" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="C110" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="D110" s="1" t="n">
+      <c r="F110" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="E110" s="1" t="n">
+      <c r="G110" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="F110" s="1" t="n">
+      <c r="H110" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="I110" s="1" t="n">
         <v>225</v>
       </c>
-      <c r="G110" s="1" t="n">
+      <c r="J110" s="1" t="n">
         <v>334</v>
       </c>
-      <c r="H110" s="1" t="n">
+      <c r="K110" s="1" t="n">
         <v>342</v>
       </c>
-      <c r="I110" s="1" t="n">
-        <v>351</v>
-      </c>
-      <c r="J110" s="1" t="n">
+      <c r="L110" s="1" t="n">
         <v>426</v>
       </c>
-      <c r="K110" s="1" t="n">
+      <c r="M110" s="1" t="n">
         <v>480</v>
       </c>
-      <c r="L110" s="1" t="n">
-        <v>494</v>
-      </c>
-      <c r="M110" s="1" t="n">
+      <c r="N110" s="1" t="n">
         <v>541</v>
-      </c>
-      <c r="N110" s="1" t="n">
-        <v>549</v>
       </c>
       <c r="O110" s="1" t="n">
         <v>565</v>
@@ -16452,49 +16452,49 @@
         <v>605</v>
       </c>
       <c r="Q110" s="1" t="n">
+        <v>636</v>
+      </c>
+      <c r="R110" s="1" t="n">
+        <v>657</v>
+      </c>
+      <c r="S110" s="1" t="n">
+        <v>678</v>
+      </c>
+      <c r="T110" s="1" t="n">
+        <v>725</v>
+      </c>
+      <c r="U110" s="1" t="n">
+        <v>872</v>
+      </c>
+      <c r="V110" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="W110" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="X110" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="Y110" s="1" t="n">
+        <v>494</v>
+      </c>
+      <c r="Z110" s="1" t="n">
+        <v>549</v>
+      </c>
+      <c r="AA110" s="1" t="n">
+        <v>584</v>
+      </c>
+      <c r="AB110" s="1" t="n">
         <v>625</v>
       </c>
-      <c r="R110" s="1" t="n">
-        <v>636</v>
-      </c>
-      <c r="S110" s="1" t="n">
-        <v>657</v>
-      </c>
-      <c r="T110" s="1" t="n">
-        <v>678</v>
-      </c>
-      <c r="U110" s="1" t="n">
+      <c r="AC110" s="1" t="n">
         <v>712</v>
       </c>
-      <c r="V110" s="1" t="n">
-        <v>725</v>
-      </c>
-      <c r="W110" s="1" t="n">
+      <c r="AD110" s="1" t="n">
         <v>864</v>
       </c>
-      <c r="X110" s="1" t="n">
+      <c r="AE110" s="1" t="n">
         <v>871</v>
-      </c>
-      <c r="Y110" s="1" t="n">
-        <v>872</v>
-      </c>
-      <c r="Z110" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="AA110" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="AB110" s="1" t="n">
-        <v>214</v>
-      </c>
-      <c r="AC110" s="1" t="n">
-        <v>229</v>
-      </c>
-      <c r="AD110" s="1" t="n">
-        <v>471</v>
-      </c>
-      <c r="AE110" s="1" t="n">
-        <v>584</v>
       </c>
     </row>
     <row r="111">
@@ -16520,107 +16520,107 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="L111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="P111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="R111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="T111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 2</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 3</t>
         </is>
       </c>
       <c r="W111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 3</t>
         </is>
       </c>
       <c r="X111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 3</t>
         </is>
       </c>
       <c r="Y111" t="inlineStr">
         <is>
-          <t>Cat 1</t>
+          <t>Cat 3</t>
         </is>
       </c>
       <c r="Z111" t="inlineStr">
@@ -16695,152 +16695,152 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
+          <t>11/17 (64.7%)</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
           <t>9/17 (52.9%)</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr">
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>5/17 (29.4%)</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>7/17 (41.2%)</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>8/17 (47.1%)</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>3/17 (17.6%)</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>5/17 (29.4%)</t>
+        </is>
+      </c>
+      <c r="P113" t="inlineStr">
+        <is>
+          <t>3/17 (17.6%)</t>
+        </is>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>5/17 (29.4%)</t>
+        </is>
+      </c>
+      <c r="T113" t="inlineStr">
+        <is>
+          <t>5/17 (29.4%)</t>
+        </is>
+      </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="V113" t="inlineStr">
         <is>
           <t>4/17 (23.5%)</t>
         </is>
       </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>11/17 (64.7%)</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>1/17 (5.9%)</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>1/17 (5.9%)</t>
-        </is>
-      </c>
-      <c r="G113" t="inlineStr">
+      <c r="W113" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="X113" t="inlineStr">
         <is>
           <t>8/17 (47.1%)</t>
         </is>
       </c>
-      <c r="H113" t="inlineStr">
-        <is>
-          <t>2/17 (11.8%)</t>
-        </is>
-      </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>11/17 (64.7%)</t>
-        </is>
-      </c>
-      <c r="J113" t="inlineStr">
+      <c r="Y113" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="Z113" t="inlineStr">
+        <is>
+          <t>10/17 (58.8%)</t>
+        </is>
+      </c>
+      <c r="AA113" t="inlineStr">
         <is>
           <t>6/17 (35.3%)</t>
         </is>
       </c>
-      <c r="K113" t="inlineStr">
+      <c r="AB113" t="inlineStr">
+        <is>
+          <t>7/17 (41.2%)</t>
+        </is>
+      </c>
+      <c r="AC113" t="inlineStr">
         <is>
           <t>4/17 (23.5%)</t>
         </is>
       </c>
-      <c r="L113" t="inlineStr">
-        <is>
-          <t>2/17 (11.8%)</t>
-        </is>
-      </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>3/17 (17.6%)</t>
-        </is>
-      </c>
-      <c r="N113" t="inlineStr">
-        <is>
-          <t>14/17 (82.4%)</t>
-        </is>
-      </c>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>9/17 (52.9%)</t>
-        </is>
-      </c>
-      <c r="P113" t="inlineStr">
-        <is>
-          <t>7/17 (41.2%)</t>
-        </is>
-      </c>
-      <c r="Q113" t="inlineStr">
+      <c r="AD113" t="inlineStr">
         <is>
           <t>10/17 (58.8%)</t>
         </is>
       </c>
-      <c r="R113" t="inlineStr">
-        <is>
-          <t>1/17 (5.9%)</t>
-        </is>
-      </c>
-      <c r="S113" t="inlineStr">
-        <is>
-          <t>4/17 (23.5%)</t>
-        </is>
-      </c>
-      <c r="T113" t="inlineStr">
-        <is>
-          <t>7/17 (41.2%)</t>
-        </is>
-      </c>
-      <c r="U113" t="inlineStr">
+      <c r="AE113" t="inlineStr">
         <is>
           <t>5/17 (29.4%)</t>
-        </is>
-      </c>
-      <c r="V113" t="inlineStr">
-        <is>
-          <t>9/17 (52.9%)</t>
-        </is>
-      </c>
-      <c r="W113" t="inlineStr">
-        <is>
-          <t>11/17 (64.7%)</t>
-        </is>
-      </c>
-      <c r="X113" t="inlineStr">
-        <is>
-          <t>6/17 (35.3%)</t>
-        </is>
-      </c>
-      <c r="Y113" t="inlineStr">
-        <is>
-          <t>1/17 (5.9%)</t>
-        </is>
-      </c>
-      <c r="Z113" t="inlineStr">
-        <is>
-          <t>7/17 (41.2%)</t>
-        </is>
-      </c>
-      <c r="AA113" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="AB113" t="inlineStr">
-        <is>
-          <t>4/17 (23.5%)</t>
-        </is>
-      </c>
-      <c r="AC113" t="inlineStr">
-        <is>
-          <t>6/17 (35.3%)</t>
-        </is>
-      </c>
-      <c r="AD113" t="inlineStr">
-        <is>
-          <t>3/17 (17.6%)</t>
-        </is>
-      </c>
-      <c r="AE113" t="inlineStr">
-        <is>
-          <t>3/17 (17.6%)</t>
         </is>
       </c>
     </row>
@@ -16852,152 +16852,152 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>0.2877</t>
+          <t>0.8965</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>0.0209</t>
+          <t>0.3952</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>0.9006</t>
+          <t>0.3743</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>0.0004</t>
+          <t>0.0271</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>0.0003</t>
+          <t>0.1189</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>0.2478</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>0.0004</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>0.7303</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>0.0194</t>
+          <t>0.0032</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>0.0096</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="L114" t="inlineStr">
         <is>
-          <t>0.0003</t>
+          <t>0.0014</t>
         </is>
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>0.0022</t>
+          <t>0.0014</t>
         </is>
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>1.3636</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
         <is>
-          <t>0.4558</t>
+          <t>0.0710</t>
         </is>
       </c>
       <c r="P114" t="inlineStr">
         <is>
-          <t>0.3178</t>
+          <t>0.0463</t>
         </is>
       </c>
       <c r="Q114" t="inlineStr">
         <is>
-          <t>0.4446</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="R114" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="S114" t="inlineStr">
         <is>
-          <t>0.0032</t>
+          <t>0.0113</t>
         </is>
       </c>
       <c r="T114" t="inlineStr">
         <is>
-          <t>0.2886</t>
+          <t>0.0513</t>
         </is>
       </c>
       <c r="U114" t="inlineStr">
         <is>
-          <t>1.2359</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>0.5820</t>
+          <t>0.0328</t>
         </is>
       </c>
       <c r="W114" t="inlineStr">
         <is>
-          <t>0.4482</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="X114" t="inlineStr">
         <is>
-          <t>0.3658</t>
+          <t>0.3917</t>
         </is>
       </c>
       <c r="Y114" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="Z114" t="inlineStr">
         <is>
-          <t>0.0746</t>
+          <t>0.1248</t>
         </is>
       </c>
       <c r="AA114" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0684</t>
         </is>
       </c>
       <c r="AB114" t="inlineStr">
         <is>
-          <t>0.0743</t>
+          <t>0.0887</t>
         </is>
       </c>
       <c r="AC114" t="inlineStr">
         <is>
-          <t>0.1092</t>
+          <t>0.0927</t>
         </is>
       </c>
       <c r="AD114" t="inlineStr">
         <is>
-          <t>0.0366</t>
+          <t>0.0898</t>
         </is>
       </c>
       <c r="AE114" t="inlineStr">
         <is>
-          <t>0.0255</t>
+          <t>0.0389</t>
         </is>
       </c>
     </row>
@@ -17009,152 +17009,152 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
+          <t>11/32 (34.4%)</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>14/32 (43.8%)</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
           <t>7/32 (21.9%)</t>
         </is>
       </c>
-      <c r="C115" t="inlineStr">
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>12/32 (37.5%)</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>15/32 (46.9%)</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>1/32 (3.1%)</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
         <is>
           <t>2/32 (6.2%)</t>
         </is>
       </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>16/32 (50.0%)</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>0/32 (0.0%)</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>0/32 (0.0%)</t>
-        </is>
-      </c>
-      <c r="G115" t="inlineStr">
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>1/32 (3.1%)</t>
+        </is>
+      </c>
+      <c r="J115" t="inlineStr">
         <is>
           <t>6/32 (18.8%)</t>
         </is>
       </c>
-      <c r="H115" t="inlineStr">
-        <is>
-          <t>0/32 (0.0%)</t>
-        </is>
-      </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>16/32 (50.0%)</t>
-        </is>
-      </c>
-      <c r="J115" t="inlineStr">
-        <is>
-          <t>6/32 (18.8%)</t>
-        </is>
-      </c>
       <c r="K115" t="inlineStr">
         <is>
+          <t>2/32 (6.2%)</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>8/32 (25.0%)</t>
+        </is>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
           <t>5/32 (15.6%)</t>
         </is>
       </c>
-      <c r="L115" t="inlineStr">
-        <is>
-          <t>0/32 (0.0%)</t>
-        </is>
-      </c>
-      <c r="M115" t="inlineStr">
-        <is>
-          <t>0/32 (0.0%)</t>
-        </is>
-      </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>14/32 (43.8%)</t>
+          <t>2/32 (6.2%)</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
         <is>
+          <t>9/32 (28.1%)</t>
+        </is>
+      </c>
+      <c r="P115" t="inlineStr">
+        <is>
+          <t>7/32 (21.9%)</t>
+        </is>
+      </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>1/32 (3.1%)</t>
+        </is>
+      </c>
+      <c r="R115" t="inlineStr">
+        <is>
+          <t>5/32 (15.6%)</t>
+        </is>
+      </c>
+      <c r="S115" t="inlineStr">
+        <is>
+          <t>11/32 (34.4%)</t>
+        </is>
+      </c>
+      <c r="T115" t="inlineStr">
+        <is>
           <t>8/32 (25.0%)</t>
         </is>
       </c>
-      <c r="P115" t="inlineStr">
-        <is>
-          <t>6/32 (18.8%)</t>
-        </is>
-      </c>
-      <c r="Q115" t="inlineStr">
+      <c r="U115" t="inlineStr">
+        <is>
+          <t>1/32 (3.1%)</t>
+        </is>
+      </c>
+      <c r="V115" t="inlineStr">
+        <is>
+          <t>10/32 (31.2%)</t>
+        </is>
+      </c>
+      <c r="W115" t="inlineStr">
+        <is>
+          <t>3/32 (9.4%)</t>
+        </is>
+      </c>
+      <c r="X115" t="inlineStr">
         <is>
           <t>8/32 (25.0%)</t>
         </is>
       </c>
-      <c r="R115" t="inlineStr">
-        <is>
-          <t>0/32 (0.0%)</t>
-        </is>
-      </c>
-      <c r="S115" t="inlineStr">
-        <is>
-          <t>2/32 (6.2%)</t>
-        </is>
-      </c>
-      <c r="T115" t="inlineStr">
-        <is>
-          <t>13/32 (40.6%)</t>
-        </is>
-      </c>
-      <c r="U115" t="inlineStr">
-        <is>
-          <t>6/32 (18.8%)</t>
-        </is>
-      </c>
-      <c r="V115" t="inlineStr">
-        <is>
-          <t>6/32 (18.8%)</t>
-        </is>
-      </c>
-      <c r="W115" t="inlineStr">
-        <is>
-          <t>16/32 (50.0%)</t>
-        </is>
-      </c>
-      <c r="X115" t="inlineStr">
+      <c r="Y115" t="inlineStr">
+        <is>
+          <t>1/32 (3.1%)</t>
+        </is>
+      </c>
+      <c r="Z115" t="inlineStr">
+        <is>
+          <t>17/32 (53.1%)</t>
+        </is>
+      </c>
+      <c r="AA115" t="inlineStr">
+        <is>
+          <t>7/32 (21.9%)</t>
+        </is>
+      </c>
+      <c r="AB115" t="inlineStr">
+        <is>
+          <t>9/32 (28.1%)</t>
+        </is>
+      </c>
+      <c r="AC115" t="inlineStr">
+        <is>
+          <t>7/32 (21.9%)</t>
+        </is>
+      </c>
+      <c r="AD115" t="inlineStr">
+        <is>
+          <t>17/32 (53.1%)</t>
+        </is>
+      </c>
+      <c r="AE115" t="inlineStr">
         <is>
           <t>8/32 (25.0%)</t>
-        </is>
-      </c>
-      <c r="Y115" t="inlineStr">
-        <is>
-          <t>0/32 (0.0%)</t>
-        </is>
-      </c>
-      <c r="Z115" t="inlineStr">
-        <is>
-          <t>5/32 (15.6%)</t>
-        </is>
-      </c>
-      <c r="AA115" t="inlineStr">
-        <is>
-          <t>0/32 (0.0%)</t>
-        </is>
-      </c>
-      <c r="AB115" t="inlineStr">
-        <is>
-          <t>8/32 (25.0%)</t>
-        </is>
-      </c>
-      <c r="AC115" t="inlineStr">
-        <is>
-          <t>12/32 (37.5%)</t>
-        </is>
-      </c>
-      <c r="AD115" t="inlineStr">
-        <is>
-          <t>6/32 (18.8%)</t>
-        </is>
-      </c>
-      <c r="AE115" t="inlineStr">
-        <is>
-          <t>7/32 (21.9%)</t>
         </is>
       </c>
     </row>
@@ -17166,152 +17166,152 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>0.0181</t>
+          <t>0.1859</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>0.0020</t>
+          <t>0.4440</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>0.5326</t>
+          <t>0.0767</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.1321</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.6210</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>0.0059</t>
+          <t>0.0002</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0008</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
         <is>
-          <t>0.2684</t>
+          <t>0.0001</t>
         </is>
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>0.0064</t>
+          <t>0.1279</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
         <is>
-          <t>0.0032</t>
+          <t>0.0002</t>
         </is>
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0122</t>
         </is>
       </c>
       <c r="M116" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0056</t>
         </is>
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>0.1728</t>
+          <t>0.0011</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
         <is>
-          <t>0.0474</t>
+          <t>0.2458</t>
         </is>
       </c>
       <c r="P116" t="inlineStr">
         <is>
-          <t>0.0347</t>
+          <t>0.1753</t>
         </is>
       </c>
       <c r="Q116" t="inlineStr">
         <is>
-          <t>0.0553</t>
+          <t>0.0001</t>
         </is>
       </c>
       <c r="R116" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0023</t>
         </is>
       </c>
       <c r="S116" t="inlineStr">
         <is>
-          <t>0.0010</t>
+          <t>0.1714</t>
         </is>
       </c>
       <c r="T116" t="inlineStr">
         <is>
-          <t>0.0304</t>
+          <t>0.3120</t>
         </is>
       </c>
       <c r="U116" t="inlineStr">
         <is>
-          <t>0.1555</t>
+          <t>0.0001</t>
         </is>
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>0.0278</t>
+          <t>0.0462</t>
         </is>
       </c>
       <c r="W116" t="inlineStr">
         <is>
-          <t>0.0463</t>
+          <t>0.0048</t>
         </is>
       </c>
       <c r="X116" t="inlineStr">
         <is>
-          <t>0.0491</t>
+          <t>0.3298</t>
         </is>
       </c>
       <c r="Y116" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0001</t>
         </is>
       </c>
       <c r="Z116" t="inlineStr">
         <is>
-          <t>0.0072</t>
+          <t>0.5495</t>
         </is>
       </c>
       <c r="AA116" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0929</t>
         </is>
       </c>
       <c r="AB116" t="inlineStr">
         <is>
-          <t>0.2834</t>
+          <t>0.1332</t>
         </is>
       </c>
       <c r="AC116" t="inlineStr">
         <is>
-          <t>0.1405</t>
+          <t>0.3511</t>
         </is>
       </c>
       <c r="AD116" t="inlineStr">
         <is>
-          <t>0.0369</t>
+          <t>0.2125</t>
         </is>
       </c>
       <c r="AE116" t="inlineStr">
         <is>
-          <t>0.0225</t>
+          <t>0.1089</t>
         </is>
       </c>
     </row>
@@ -17323,152 +17323,152 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
+          <t>9/21 (42.9%)</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>10/21 (47.6%)</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>6/21 (28.6%)</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>10/21 (47.6%)</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>9/21 (42.9%)</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>6/21 (28.6%)</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>5/21 (23.8%)</t>
+        </is>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>4/21 (19.0%)</t>
+        </is>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>7/21 (33.3%)</t>
+        </is>
+      </c>
+      <c r="P117" t="inlineStr">
+        <is>
+          <t>5/21 (23.8%)</t>
+        </is>
+      </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="R117" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="S117" t="inlineStr">
+        <is>
+          <t>11/21 (52.4%)</t>
+        </is>
+      </c>
+      <c r="T117" t="inlineStr">
+        <is>
+          <t>6/21 (28.6%)</t>
+        </is>
+      </c>
+      <c r="U117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="V117" t="inlineStr">
+        <is>
+          <t>9/21 (42.9%)</t>
+        </is>
+      </c>
+      <c r="W117" t="inlineStr">
+        <is>
+          <t>3/21 (14.3%)</t>
+        </is>
+      </c>
+      <c r="X117" t="inlineStr">
+        <is>
+          <t>7/21 (33.3%)</t>
+        </is>
+      </c>
+      <c r="Y117" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="Z117" t="inlineStr">
+        <is>
           <t>13/21 (61.9%)</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
+      <c r="AA117" t="inlineStr">
+        <is>
+          <t>6/21 (28.6%)</t>
+        </is>
+      </c>
+      <c r="AB117" t="inlineStr">
         <is>
           <t>5/21 (23.8%)</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>1/21 (4.8%)</t>
-        </is>
-      </c>
-      <c r="H117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="I117" t="inlineStr">
+      <c r="AC117" t="inlineStr">
         <is>
           <t>6/21 (28.6%)</t>
         </is>
       </c>
-      <c r="J117" t="inlineStr">
-        <is>
-          <t>2/21 (9.5%)</t>
-        </is>
-      </c>
-      <c r="K117" t="inlineStr">
-        <is>
-          <t>1/21 (4.8%)</t>
-        </is>
-      </c>
-      <c r="L117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="M117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="N117" t="inlineStr">
-        <is>
-          <t>12/21 (57.1%)</t>
-        </is>
-      </c>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>4/21 (19.0%)</t>
-        </is>
-      </c>
-      <c r="P117" t="inlineStr">
-        <is>
-          <t>2/21 (9.5%)</t>
-        </is>
-      </c>
-      <c r="Q117" t="inlineStr">
-        <is>
-          <t>3/21 (14.3%)</t>
-        </is>
-      </c>
-      <c r="R117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="S117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="T117" t="inlineStr">
-        <is>
-          <t>7/21 (33.3%)</t>
-        </is>
-      </c>
-      <c r="U117" t="inlineStr">
-        <is>
-          <t>6/21 (28.6%)</t>
-        </is>
-      </c>
-      <c r="V117" t="inlineStr">
-        <is>
-          <t>4/21 (19.0%)</t>
-        </is>
-      </c>
-      <c r="W117" t="inlineStr">
+      <c r="AD117" t="inlineStr">
         <is>
           <t>13/21 (61.9%)</t>
         </is>
       </c>
-      <c r="X117" t="inlineStr">
-        <is>
-          <t>4/21 (19.0%)</t>
-        </is>
-      </c>
-      <c r="Y117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="Z117" t="inlineStr">
-        <is>
-          <t>11/21 (52.4%)</t>
-        </is>
-      </c>
-      <c r="AA117" t="inlineStr">
-        <is>
-          <t>3/21 (14.3%)</t>
-        </is>
-      </c>
-      <c r="AB117" t="inlineStr">
-        <is>
-          <t>11/21 (52.4%)</t>
-        </is>
-      </c>
-      <c r="AC117" t="inlineStr">
-        <is>
-          <t>13/21 (61.9%)</t>
-        </is>
-      </c>
-      <c r="AD117" t="inlineStr">
-        <is>
-          <t>9/21 (42.9%)</t>
-        </is>
-      </c>
       <c r="AE117" t="inlineStr">
         <is>
-          <t>9/21 (42.9%)</t>
+          <t>5/21 (23.8%)</t>
         </is>
       </c>
     </row>
@@ -17480,152 +17480,152 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>0.0518</t>
+          <t>0.4792</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.1133</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>0.0317</t>
+          <t>0.1109</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0889</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.5297</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>0.0010</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0007</t>
         </is>
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>0.1097</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="J118" t="inlineStr">
         <is>
-          <t>0.0009</t>
+          <t>0.0131</t>
         </is>
       </c>
       <c r="K118" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="L118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0066</t>
         </is>
       </c>
       <c r="M118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0032</t>
         </is>
       </c>
       <c r="N118" t="inlineStr">
         <is>
-          <t>0.0762</t>
+          <t>0.0002</t>
         </is>
       </c>
       <c r="O118" t="inlineStr">
         <is>
-          <t>0.0294</t>
+          <t>0.0386</t>
         </is>
       </c>
       <c r="P118" t="inlineStr">
         <is>
-          <t>0.0848</t>
+          <t>0.0903</t>
         </is>
       </c>
       <c r="Q118" t="inlineStr">
         <is>
-          <t>0.0457</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="R118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0005</t>
         </is>
       </c>
       <c r="S118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0228</t>
         </is>
       </c>
       <c r="T118" t="inlineStr">
         <is>
-          <t>0.0131</t>
+          <t>0.0383</t>
         </is>
       </c>
       <c r="U118" t="inlineStr">
         <is>
-          <t>0.0098</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>0.0418</t>
+          <t>0.0779</t>
         </is>
       </c>
       <c r="W118" t="inlineStr">
         <is>
-          <t>0.1689</t>
+          <t>0.0127</t>
         </is>
       </c>
       <c r="X118" t="inlineStr">
         <is>
-          <t>0.0073</t>
+          <t>1.1824</t>
         </is>
       </c>
       <c r="Y118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0002</t>
         </is>
       </c>
       <c r="Z118" t="inlineStr">
         <is>
-          <t>0.1035</t>
+          <t>0.5050</t>
         </is>
       </c>
       <c r="AA118" t="inlineStr">
         <is>
-          <t>0.0019</t>
+          <t>0.1086</t>
         </is>
       </c>
       <c r="AB118" t="inlineStr">
         <is>
-          <t>1.5101</t>
+          <t>0.2151</t>
         </is>
       </c>
       <c r="AC118" t="inlineStr">
         <is>
-          <t>1.1856</t>
+          <t>0.6372</t>
         </is>
       </c>
       <c r="AD118" t="inlineStr">
         <is>
-          <t>0.4448</t>
+          <t>0.2058</t>
         </is>
       </c>
       <c r="AE118" t="inlineStr">
         <is>
-          <t>0.2507</t>
+          <t>0.1810</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Reinstating the directories and notebooks
</commit_message>
<xml_diff>
--- a/data/feature_analysis_results.xlsx
+++ b/data/feature_analysis_results.xlsx
@@ -8460,10 +8460,10 @@
         </is>
       </c>
       <c r="B62" s="1" t="n">
-        <v>201</v>
+        <v>23</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>229</v>
+        <v>91</v>
       </c>
       <c r="D62" s="1" t="n">
         <v>334</v>
@@ -8472,64 +8472,64 @@
         <v>342</v>
       </c>
       <c r="F62" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="G62" s="1" t="n">
+        <v>375</v>
+      </c>
+      <c r="H62" s="1" t="n">
         <v>410</v>
       </c>
-      <c r="G62" s="1" t="n">
-        <v>471</v>
-      </c>
-      <c r="H62" s="1" t="n">
+      <c r="I62" s="1" t="n">
+        <v>494</v>
+      </c>
+      <c r="J62" s="1" t="n">
+        <v>541</v>
+      </c>
+      <c r="K62" s="1" t="n">
         <v>549</v>
       </c>
-      <c r="I62" s="1" t="n">
+      <c r="L62" s="1" t="n">
+        <v>565</v>
+      </c>
+      <c r="M62" s="1" t="n">
         <v>625</v>
       </c>
-      <c r="J62" s="1" t="n">
+      <c r="N62" s="1" t="n">
         <v>678</v>
       </c>
-      <c r="K62" s="1" t="n">
+      <c r="O62" s="1" t="n">
         <v>712</v>
       </c>
-      <c r="L62" s="1" t="n">
+      <c r="P62" s="1" t="n">
+        <v>725</v>
+      </c>
+      <c r="Q62" s="1" t="n">
         <v>799</v>
       </c>
-      <c r="M62" s="1" t="n">
+      <c r="R62" s="1" t="n">
+        <v>864</v>
+      </c>
+      <c r="S62" s="1" t="n">
         <v>871</v>
-      </c>
-      <c r="N62" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="O62" s="1" t="n">
-        <v>351</v>
-      </c>
-      <c r="P62" s="1" t="n">
-        <v>375</v>
-      </c>
-      <c r="Q62" s="1" t="n">
-        <v>541</v>
-      </c>
-      <c r="R62" s="1" t="n">
-        <v>565</v>
-      </c>
-      <c r="S62" s="1" t="n">
-        <v>725</v>
       </c>
       <c r="T62" s="1" t="n">
         <v>863</v>
       </c>
       <c r="U62" s="1" t="n">
-        <v>864</v>
+        <v>201</v>
       </c>
       <c r="V62" s="1" t="n">
-        <v>91</v>
+        <v>214</v>
       </c>
       <c r="W62" s="1" t="n">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="X62" s="1" t="n">
         <v>408</v>
       </c>
       <c r="Y62" s="1" t="n">
-        <v>494</v>
+        <v>471</v>
       </c>
       <c r="Z62" s="1" t="n">
         <v>526</v>
@@ -8606,42 +8606,42 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="T63" t="inlineStr">
+        <is>
           <t>Cat 2</t>
         </is>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>Cat 2</t>
-        </is>
-      </c>
-      <c r="P63" t="inlineStr">
-        <is>
-          <t>Cat 2</t>
-        </is>
-      </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>Cat 2</t>
-        </is>
-      </c>
-      <c r="R63" t="inlineStr">
-        <is>
-          <t>Cat 2</t>
-        </is>
-      </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>Cat 2</t>
-        </is>
-      </c>
-      <c r="T63" t="inlineStr">
-        <is>
-          <t>Cat 2</t>
-        </is>
-      </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 3</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
@@ -8712,117 +8712,117 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>1/17 (5.9%)</t>
+          <t>9/17 (52.9%)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
+          <t>11/17 (64.7%)</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>8/17 (47.1%)</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2/17 (11.8%)</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>11/17 (64.7%)</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>11/17 (64.7%)</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>2/17 (11.8%)</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>2/17 (11.8%)</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>3/17 (17.6%)</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>14/17 (82.4%)</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>9/17 (52.9%)</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>10/17 (58.8%)</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>7/17 (41.2%)</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
           <t>5/17 (29.4%)</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>4/17 (23.5%)</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>1/17 (5.9%)</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>1/17 (5.9%)</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>9/17 (52.9%)</t>
+        </is>
+      </c>
+      <c r="Q65" t="inlineStr">
         <is>
           <t>2/17 (11.8%)</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>4/17 (23.5%)</t>
-        </is>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>5/17 (29.4%)</t>
-        </is>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>3/17 (17.6%)</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>2/17 (11.8%)</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>1/17 (5.9%)</t>
-        </is>
-      </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>2/17 (11.8%)</t>
-        </is>
-      </c>
-      <c r="N65" t="inlineStr">
-        <is>
-          <t>2/17 (11.8%)</t>
-        </is>
-      </c>
-      <c r="O65" t="inlineStr">
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>11/17 (64.7%)</t>
+        </is>
+      </c>
+      <c r="S65" t="inlineStr">
         <is>
           <t>6/17 (35.3%)</t>
         </is>
       </c>
-      <c r="P65" t="inlineStr">
-        <is>
-          <t>3/17 (17.6%)</t>
-        </is>
-      </c>
-      <c r="Q65" t="inlineStr">
+      <c r="T65" t="inlineStr">
+        <is>
+          <t>10/17 (58.8%)</t>
+        </is>
+      </c>
+      <c r="U65" t="inlineStr">
         <is>
           <t>0/17 (0.0%)</t>
         </is>
       </c>
-      <c r="R65" t="inlineStr">
-        <is>
-          <t>3/17 (17.6%)</t>
-        </is>
-      </c>
-      <c r="S65" t="inlineStr">
-        <is>
-          <t>1/17 (5.9%)</t>
-        </is>
-      </c>
-      <c r="T65" t="inlineStr">
-        <is>
-          <t>7/17 (41.2%)</t>
-        </is>
-      </c>
-      <c r="U65" t="inlineStr">
-        <is>
-          <t>2/17 (11.8%)</t>
-        </is>
-      </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>7/17 (41.2%)</t>
+          <t>0/17 (0.0%)</t>
         </is>
       </c>
       <c r="W65" t="inlineStr">
         <is>
-          <t>4/17 (23.5%)</t>
+          <t>0/17 (0.0%)</t>
         </is>
       </c>
       <c r="X65" t="inlineStr">
         <is>
-          <t>7/17 (41.2%)</t>
+          <t>0/17 (0.0%)</t>
         </is>
       </c>
       <c r="Y65" t="inlineStr">
@@ -8832,12 +8832,12 @@
       </c>
       <c r="Z65" t="inlineStr">
         <is>
-          <t>3/17 (17.6%)</t>
+          <t>0/17 (0.0%)</t>
         </is>
       </c>
       <c r="AA65" t="inlineStr">
         <is>
-          <t>2/17 (11.8%)</t>
+          <t>0/17 (0.0%)</t>
         </is>
       </c>
     </row>
@@ -8849,117 +8849,117 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>0.0006</t>
+          <t>0.2877</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.0213</t>
+          <t>0.9006</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>0.2403</t>
+          <t>0.2478</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
+          <t>0.0004</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>0.7303</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>0.7887</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
           <t>0.0002</t>
         </is>
       </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>0.0001</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>0.3676</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>0.6593</t>
-        </is>
-      </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>0.2304</t>
+          <t>0.0003</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>0.2794</t>
+          <t>0.0022</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>0.6123</t>
+          <t>1.3636</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.4559</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>0.1833</t>
+          <t>0.4446</t>
         </is>
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>0.0026</t>
+          <t>0.2886</t>
         </is>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>0.3639</t>
+          <t>1.2359</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>0.0538</t>
+          <t>0.5820</t>
         </is>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0002</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
         <is>
-          <t>0.0133</t>
+          <t>0.4482</t>
         </is>
       </c>
       <c r="S66" t="inlineStr">
         <is>
-          <t>0.0005</t>
+          <t>0.3658</t>
         </is>
       </c>
       <c r="T66" t="inlineStr">
         <is>
-          <t>0.2060</t>
+          <t>0.4485</t>
         </is>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>0.0093</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>0.5332</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="W66" t="inlineStr">
         <is>
-          <t>0.4934</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="X66" t="inlineStr">
         <is>
-          <t>0.0624</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="Y66" t="inlineStr">
@@ -8969,12 +8969,12 @@
       </c>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>0.0909</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="AA66" t="inlineStr">
         <is>
-          <t>0.1435</t>
+          <t>0.0000</t>
         </is>
       </c>
     </row>
@@ -8986,132 +8986,132 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>1/32 (3.1%)</t>
+          <t>0/32 (0.0%)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
+          <t>16/32 (50.0%)</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>16/32 (50.0%)</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="T67" t="inlineStr">
+        <is>
+          <t>19/32 (59.4%)</t>
+        </is>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>8/32 (25.0%)</t>
+        </is>
+      </c>
+      <c r="W67" t="inlineStr">
+        <is>
           <t>12/32 (37.5%)</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>3/32 (9.4%)</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>1/32 (3.1%)</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>1/32 (3.1%)</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>3/32 (9.4%)</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>8/32 (25.0%)</t>
-        </is>
-      </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>4/32 (12.5%)</t>
-        </is>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>3/32 (9.4%)</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>2/32 (6.2%)</t>
-        </is>
-      </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>1/32 (3.1%)</t>
-        </is>
-      </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>3/32 (9.4%)</t>
-        </is>
-      </c>
-      <c r="N67" t="inlineStr">
-        <is>
-          <t>5/32 (15.6%)</t>
-        </is>
-      </c>
-      <c r="O67" t="inlineStr">
+      <c r="X67" t="inlineStr">
         <is>
           <t>14/32 (43.8%)</t>
         </is>
       </c>
-      <c r="P67" t="inlineStr">
-        <is>
-          <t>6/32 (18.8%)</t>
-        </is>
-      </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>2/32 (6.2%)</t>
-        </is>
-      </c>
-      <c r="R67" t="inlineStr">
-        <is>
-          <t>4/32 (12.5%)</t>
-        </is>
-      </c>
-      <c r="S67" t="inlineStr">
-        <is>
-          <t>6/32 (18.8%)</t>
-        </is>
-      </c>
-      <c r="T67" t="inlineStr">
-        <is>
-          <t>14/32 (43.8%)</t>
-        </is>
-      </c>
-      <c r="U67" t="inlineStr">
-        <is>
-          <t>6/32 (18.8%)</t>
-        </is>
-      </c>
-      <c r="V67" t="inlineStr">
-        <is>
-          <t>12/32 (37.5%)</t>
-        </is>
-      </c>
-      <c r="W67" t="inlineStr">
-        <is>
-          <t>7/32 (21.9%)</t>
-        </is>
-      </c>
-      <c r="X67" t="inlineStr">
-        <is>
-          <t>11/32 (34.4%)</t>
-        </is>
-      </c>
       <c r="Y67" t="inlineStr">
         <is>
-          <t>1/32 (3.1%)</t>
+          <t>0/32 (0.0%)</t>
         </is>
       </c>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>6/32 (18.8%)</t>
+          <t>0/32 (0.0%)</t>
         </is>
       </c>
       <c r="AA67" t="inlineStr">
         <is>
-          <t>3/32 (9.4%)</t>
+          <t>0/32 (0.0%)</t>
         </is>
       </c>
     </row>
@@ -9123,52 +9123,52 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>0.0005</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>0.2524</t>
+          <t>0.5326</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0.0006</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.2684</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>0.0656</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>0.3253</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>0.0007</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>0.0007</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>0.0009</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
@@ -9178,77 +9178,77 @@
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>0.0016</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>0.1118</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>0.4086</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>0.3656</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>0.0011</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
         <is>
-          <t>0.2257</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="S68" t="inlineStr">
         <is>
-          <t>0.2992</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="T68" t="inlineStr">
         <is>
-          <t>0.4255</t>
+          <t>0.5028</t>
         </is>
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>0.1261</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>0.2808</t>
+          <t>0.2834</t>
         </is>
       </c>
       <c r="W68" t="inlineStr">
         <is>
-          <t>0.6310</t>
+          <t>0.1405</t>
         </is>
       </c>
       <c r="X68" t="inlineStr">
         <is>
-          <t>0.0713</t>
+          <t>0.1243</t>
         </is>
       </c>
       <c r="Y68" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="Z68" t="inlineStr">
         <is>
-          <t>0.1514</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="AA68" t="inlineStr">
         <is>
-          <t>0.0094</t>
+          <t>0.0000</t>
         </is>
       </c>
     </row>
@@ -9260,17 +9260,17 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>1/21 (4.8%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>8/21 (38.1%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1/21 (4.8%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -9285,27 +9285,27 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>4/21 (19.0%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>2/21 (9.5%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>1/21 (4.8%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>1/21 (4.8%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>1/21 (4.8%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -9315,42 +9315,42 @@
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>1/21 (4.8%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>2/21 (9.5%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>7/21 (33.3%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>2/21 (9.5%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>1/21 (4.8%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
         <is>
-          <t>2/21 (9.5%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="S69" t="inlineStr">
         <is>
-          <t>2/21 (9.5%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="T69" t="inlineStr">
         <is>
-          <t>8/21 (38.1%)</t>
+          <t>0/21 (0.0%)</t>
         </is>
       </c>
       <c r="U69" t="inlineStr">
@@ -9360,32 +9360,32 @@
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>8/21 (38.1%)</t>
+          <t>11/21 (52.4%)</t>
         </is>
       </c>
       <c r="W69" t="inlineStr">
         <is>
-          <t>8/21 (38.1%)</t>
+          <t>13/21 (61.9%)</t>
         </is>
       </c>
       <c r="X69" t="inlineStr">
         <is>
+          <t>13/21 (61.9%)</t>
+        </is>
+      </c>
+      <c r="Y69" t="inlineStr">
+        <is>
           <t>9/21 (42.9%)</t>
         </is>
       </c>
-      <c r="Y69" t="inlineStr">
-        <is>
-          <t>1/21 (4.8%)</t>
-        </is>
-      </c>
       <c r="Z69" t="inlineStr">
         <is>
-          <t>6/21 (28.6%)</t>
+          <t>15/21 (71.4%)</t>
         </is>
       </c>
       <c r="AA69" t="inlineStr">
         <is>
-          <t>4/21 (19.0%)</t>
+          <t>9/21 (42.9%)</t>
         </is>
       </c>
     </row>
@@ -9397,17 +9397,17 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>0.0007</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>0.1885</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>0.0052</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -9422,27 +9422,27 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>0.0473</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>0.0745</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>0.1723</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>0.0063</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>0.5035</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -9452,77 +9452,77 @@
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>0.1453</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>0.0604</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>0.0830</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>0.0378</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>0.0002</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
         <is>
-          <t>0.0142</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="S70" t="inlineStr">
         <is>
-          <t>0.0148</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="T70" t="inlineStr">
         <is>
-          <t>0.3141</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>0.1632</t>
+          <t>0.0019</t>
         </is>
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>0.6811</t>
+          <t>1.5101</t>
         </is>
       </c>
       <c r="W70" t="inlineStr">
         <is>
-          <t>0.5811</t>
+          <t>1.1856</t>
         </is>
       </c>
       <c r="X70" t="inlineStr">
         <is>
-          <t>0.4618</t>
+          <t>0.4315</t>
         </is>
       </c>
       <c r="Y70" t="inlineStr">
         <is>
-          <t>0.0002</t>
+          <t>0.4448</t>
         </is>
       </c>
       <c r="Z70" t="inlineStr">
         <is>
-          <t>0.1842</t>
+          <t>0.4884</t>
         </is>
       </c>
       <c r="AA70" t="inlineStr">
         <is>
-          <t>0.1202</t>
+          <t>0.2507</t>
         </is>
       </c>
     </row>
@@ -15951,22 +15951,22 @@
         </is>
       </c>
       <c r="B98" s="1" t="n">
+        <v>541</v>
+      </c>
+      <c r="C98" s="1" t="n">
+        <v>549</v>
+      </c>
+      <c r="D98" s="1" t="n">
         <v>238</v>
       </c>
-      <c r="C98" s="1" t="n">
-        <v>541</v>
-      </c>
-      <c r="D98" s="1" t="n">
+      <c r="E98" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="E98" s="1" t="n">
+      <c r="F98" s="1" t="n">
         <v>201</v>
       </c>
-      <c r="F98" s="1" t="n">
+      <c r="G98" s="1" t="n">
         <v>211</v>
-      </c>
-      <c r="G98" s="1" t="n">
-        <v>549</v>
       </c>
       <c r="H98" s="1" t="n">
         <v>578</v>
@@ -16004,37 +16004,37 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 3</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 3</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 3</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 3</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 3</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 3</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 3</t>
         </is>
       </c>
     </row>
@@ -16059,32 +16059,32 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2/17 (11.8%)</t>
+          <t>3/17 (17.6%)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>2/17 (11.8%)</t>
+          <t>14/17 (82.4%)</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>15/17 (88.2%)</t>
+          <t>0/17 (0.0%)</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>1/17 (5.9%)</t>
+          <t>17/17 (100.0%)</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>1/17 (5.9%)</t>
+          <t>0/17 (0.0%)</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>10/17 (58.8%)</t>
+          <t>0/17 (0.0%)</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -16116,32 +16116,32 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>5.1452</t>
+          <t>0.0022</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>0.0015</t>
+          <t>1.3636</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>3.5077</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>0.0006</t>
+          <t>3.7249</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>0.0003</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>0.2309</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -16173,52 +16173,52 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>1/32 (3.1%)</t>
+          <t>0/32 (0.0%)</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>1/32 (3.1%)</t>
+          <t>14/32 (43.8%)</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>28/32 (87.5%)</t>
+          <t>3/32 (9.4%)</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>2/32 (6.2%)</t>
+          <t>26/32 (81.2%)</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>2/32 (6.2%)</t>
+          <t>0/32 (0.0%)</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>21/32 (65.6%)</t>
+          <t>0/32 (0.0%)</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>1/32 (3.1%)</t>
+          <t>0/32 (0.0%)</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>2/32 (6.2%)</t>
+          <t>0/32 (0.0%)</t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>2/32 (6.2%)</t>
+          <t>0/32 (0.0%)</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>1/32 (3.1%)</t>
+          <t>0/32 (0.0%)</t>
         </is>
       </c>
     </row>
@@ -16230,52 +16230,52 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>0.3389</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>0.0004</t>
+          <t>0.1728</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>6.4179</t>
+          <t>3.0723</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>0.0009</t>
+          <t>5.3619</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>0.0005</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>0.6389</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>0.0006</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>0.0007</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>0.0007</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>0.0007</t>
+          <t>0.0000</t>
         </is>
       </c>
     </row>
@@ -16292,47 +16292,47 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
+          <t>12/21 (57.1%)</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
           <t>0/21 (0.0%)</t>
         </is>
       </c>
-      <c r="D105" t="inlineStr">
+      <c r="E105" t="inlineStr">
         <is>
           <t>18/21 (85.7%)</t>
         </is>
       </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>0/21 (0.0%)</t>
+          <t>3/21 (14.3%)</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>9/21 (42.9%)</t>
+          <t>3/21 (14.3%)</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
         <is>
+          <t>2/21 (9.5%)</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>2/21 (9.5%)</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>2/21 (9.5%)</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
           <t>1/21 (4.8%)</t>
-        </is>
-      </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="J105" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
         </is>
       </c>
     </row>
@@ -16349,47 +16349,47 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0762</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>5.5161</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>6.9495</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0019</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>0.2830</t>
+          <t>0.0009</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.0011</t>
         </is>
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0011</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0011</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0011</t>
         </is>
       </c>
     </row>
@@ -16407,43 +16407,43 @@
         </is>
       </c>
       <c r="B110" s="1" t="n">
-        <v>229</v>
+        <v>23</v>
       </c>
       <c r="C110" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="D110" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="E110" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="F110" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="G110" s="1" t="n">
+        <v>334</v>
+      </c>
+      <c r="H110" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="I110" s="1" t="n">
         <v>351</v>
       </c>
-      <c r="D110" s="1" t="n">
-        <v>471</v>
-      </c>
-      <c r="E110" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="F110" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="G110" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="H110" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="I110" s="1" t="n">
-        <v>225</v>
-      </c>
       <c r="J110" s="1" t="n">
-        <v>334</v>
+        <v>426</v>
       </c>
       <c r="K110" s="1" t="n">
-        <v>342</v>
+        <v>480</v>
       </c>
       <c r="L110" s="1" t="n">
-        <v>426</v>
+        <v>494</v>
       </c>
       <c r="M110" s="1" t="n">
-        <v>480</v>
+        <v>541</v>
       </c>
       <c r="N110" s="1" t="n">
-        <v>541</v>
+        <v>549</v>
       </c>
       <c r="O110" s="1" t="n">
         <v>565</v>
@@ -16452,49 +16452,49 @@
         <v>605</v>
       </c>
       <c r="Q110" s="1" t="n">
+        <v>625</v>
+      </c>
+      <c r="R110" s="1" t="n">
         <v>636</v>
       </c>
-      <c r="R110" s="1" t="n">
+      <c r="S110" s="1" t="n">
         <v>657</v>
       </c>
-      <c r="S110" s="1" t="n">
+      <c r="T110" s="1" t="n">
         <v>678</v>
       </c>
-      <c r="T110" s="1" t="n">
+      <c r="U110" s="1" t="n">
+        <v>712</v>
+      </c>
+      <c r="V110" s="1" t="n">
         <v>725</v>
       </c>
-      <c r="U110" s="1" t="n">
+      <c r="W110" s="1" t="n">
+        <v>864</v>
+      </c>
+      <c r="X110" s="1" t="n">
+        <v>871</v>
+      </c>
+      <c r="Y110" s="1" t="n">
         <v>872</v>
       </c>
-      <c r="V110" s="1" t="n">
+      <c r="Z110" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="W110" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="X110" s="1" t="n">
+      <c r="AA110" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="AB110" s="1" t="n">
         <v>214</v>
       </c>
-      <c r="Y110" s="1" t="n">
-        <v>494</v>
-      </c>
-      <c r="Z110" s="1" t="n">
-        <v>549</v>
-      </c>
-      <c r="AA110" s="1" t="n">
+      <c r="AC110" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="AD110" s="1" t="n">
+        <v>471</v>
+      </c>
+      <c r="AE110" s="1" t="n">
         <v>584</v>
-      </c>
-      <c r="AB110" s="1" t="n">
-        <v>625</v>
-      </c>
-      <c r="AC110" s="1" t="n">
-        <v>712</v>
-      </c>
-      <c r="AD110" s="1" t="n">
-        <v>864</v>
-      </c>
-      <c r="AE110" s="1" t="n">
-        <v>871</v>
       </c>
     </row>
     <row r="111">
@@ -16520,107 +16520,107 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="L111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="P111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="R111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="T111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>Cat 2</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="W111" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="X111" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="Y111" t="inlineStr">
         <is>
-          <t>Cat 3</t>
+          <t>Cat 1</t>
         </is>
       </c>
       <c r="Z111" t="inlineStr">
@@ -16695,152 +16695,152 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
+          <t>9/17 (52.9%)</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>4/17 (23.5%)</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
           <t>11/17 (64.7%)</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr">
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>8/17 (47.1%)</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>2/17 (11.8%)</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>11/17 (64.7%)</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>6/17 (35.3%)</t>
+        </is>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>4/17 (23.5%)</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>2/17 (11.8%)</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>3/17 (17.6%)</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>14/17 (82.4%)</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
         <is>
           <t>9/17 (52.9%)</t>
         </is>
       </c>
-      <c r="D113" t="inlineStr">
+      <c r="P113" t="inlineStr">
+        <is>
+          <t>7/17 (41.2%)</t>
+        </is>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>10/17 (58.8%)</t>
+        </is>
+      </c>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>4/17 (23.5%)</t>
+        </is>
+      </c>
+      <c r="T113" t="inlineStr">
+        <is>
+          <t>7/17 (41.2%)</t>
+        </is>
+      </c>
+      <c r="U113" t="inlineStr">
         <is>
           <t>5/17 (29.4%)</t>
         </is>
       </c>
-      <c r="E113" t="inlineStr">
+      <c r="V113" t="inlineStr">
+        <is>
+          <t>9/17 (52.9%)</t>
+        </is>
+      </c>
+      <c r="W113" t="inlineStr">
+        <is>
+          <t>11/17 (64.7%)</t>
+        </is>
+      </c>
+      <c r="X113" t="inlineStr">
+        <is>
+          <t>6/17 (35.3%)</t>
+        </is>
+      </c>
+      <c r="Y113" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="Z113" t="inlineStr">
         <is>
           <t>7/17 (41.2%)</t>
         </is>
       </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>8/17 (47.1%)</t>
-        </is>
-      </c>
-      <c r="G113" t="inlineStr">
+      <c r="AA113" t="inlineStr">
         <is>
           <t>0/17 (0.0%)</t>
         </is>
       </c>
-      <c r="H113" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="J113" t="inlineStr">
+      <c r="AB113" t="inlineStr">
+        <is>
+          <t>4/17 (23.5%)</t>
+        </is>
+      </c>
+      <c r="AC113" t="inlineStr">
+        <is>
+          <t>6/17 (35.3%)</t>
+        </is>
+      </c>
+      <c r="AD113" t="inlineStr">
         <is>
           <t>3/17 (17.6%)</t>
         </is>
       </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="L113" t="inlineStr">
-        <is>
-          <t>1/17 (5.9%)</t>
-        </is>
-      </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>1/17 (5.9%)</t>
-        </is>
-      </c>
-      <c r="N113" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>5/17 (29.4%)</t>
-        </is>
-      </c>
-      <c r="P113" t="inlineStr">
+      <c r="AE113" t="inlineStr">
         <is>
           <t>3/17 (17.6%)</t>
-        </is>
-      </c>
-      <c r="Q113" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="R113" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="S113" t="inlineStr">
-        <is>
-          <t>5/17 (29.4%)</t>
-        </is>
-      </c>
-      <c r="T113" t="inlineStr">
-        <is>
-          <t>5/17 (29.4%)</t>
-        </is>
-      </c>
-      <c r="U113" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="V113" t="inlineStr">
-        <is>
-          <t>4/17 (23.5%)</t>
-        </is>
-      </c>
-      <c r="W113" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="X113" t="inlineStr">
-        <is>
-          <t>8/17 (47.1%)</t>
-        </is>
-      </c>
-      <c r="Y113" t="inlineStr">
-        <is>
-          <t>0/17 (0.0%)</t>
-        </is>
-      </c>
-      <c r="Z113" t="inlineStr">
-        <is>
-          <t>10/17 (58.8%)</t>
-        </is>
-      </c>
-      <c r="AA113" t="inlineStr">
-        <is>
-          <t>6/17 (35.3%)</t>
-        </is>
-      </c>
-      <c r="AB113" t="inlineStr">
-        <is>
-          <t>7/17 (41.2%)</t>
-        </is>
-      </c>
-      <c r="AC113" t="inlineStr">
-        <is>
-          <t>4/17 (23.5%)</t>
-        </is>
-      </c>
-      <c r="AD113" t="inlineStr">
-        <is>
-          <t>10/17 (58.8%)</t>
-        </is>
-      </c>
-      <c r="AE113" t="inlineStr">
-        <is>
-          <t>5/17 (29.4%)</t>
         </is>
       </c>
     </row>
@@ -16852,152 +16852,152 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>0.8965</t>
+          <t>0.2877</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>0.3952</t>
+          <t>0.0209</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>0.3743</t>
+          <t>0.9006</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>0.0271</t>
+          <t>0.0004</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>0.1189</t>
+          <t>0.0003</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.2478</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0004</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.7303</t>
         </is>
       </c>
       <c r="J114" t="inlineStr">
         <is>
+          <t>0.0194</t>
+        </is>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>0.0096</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>0.0003</t>
+        </is>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>0.0022</t>
+        </is>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>1.3636</t>
+        </is>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>0.4558</t>
+        </is>
+      </c>
+      <c r="P114" t="inlineStr">
+        <is>
+          <t>0.3178</t>
+        </is>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>0.4446</t>
+        </is>
+      </c>
+      <c r="R114" t="inlineStr">
+        <is>
+          <t>0.0001</t>
+        </is>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
           <t>0.0032</t>
         </is>
       </c>
-      <c r="K114" t="inlineStr">
-        <is>
-          <t>0.0000</t>
-        </is>
-      </c>
-      <c r="L114" t="inlineStr">
-        <is>
-          <t>0.0014</t>
-        </is>
-      </c>
-      <c r="M114" t="inlineStr">
-        <is>
-          <t>0.0014</t>
-        </is>
-      </c>
-      <c r="N114" t="inlineStr">
-        <is>
-          <t>0.0000</t>
-        </is>
-      </c>
-      <c r="O114" t="inlineStr">
-        <is>
-          <t>0.0710</t>
-        </is>
-      </c>
-      <c r="P114" t="inlineStr">
-        <is>
-          <t>0.0463</t>
-        </is>
-      </c>
-      <c r="Q114" t="inlineStr">
-        <is>
-          <t>0.0000</t>
-        </is>
-      </c>
-      <c r="R114" t="inlineStr">
-        <is>
-          <t>0.0000</t>
-        </is>
-      </c>
-      <c r="S114" t="inlineStr">
-        <is>
-          <t>0.0113</t>
-        </is>
-      </c>
       <c r="T114" t="inlineStr">
         <is>
-          <t>0.0513</t>
+          <t>0.2886</t>
         </is>
       </c>
       <c r="U114" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>1.2359</t>
         </is>
       </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>0.0328</t>
+          <t>0.5820</t>
         </is>
       </c>
       <c r="W114" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.4482</t>
         </is>
       </c>
       <c r="X114" t="inlineStr">
         <is>
-          <t>0.3917</t>
+          <t>0.3658</t>
         </is>
       </c>
       <c r="Y114" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0001</t>
         </is>
       </c>
       <c r="Z114" t="inlineStr">
         <is>
-          <t>0.1248</t>
+          <t>0.0746</t>
         </is>
       </c>
       <c r="AA114" t="inlineStr">
         <is>
-          <t>0.0684</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="AB114" t="inlineStr">
         <is>
-          <t>0.0887</t>
+          <t>0.0743</t>
         </is>
       </c>
       <c r="AC114" t="inlineStr">
         <is>
-          <t>0.0927</t>
+          <t>0.1092</t>
         </is>
       </c>
       <c r="AD114" t="inlineStr">
         <is>
-          <t>0.0898</t>
+          <t>0.0366</t>
         </is>
       </c>
       <c r="AE114" t="inlineStr">
         <is>
-          <t>0.0389</t>
+          <t>0.0255</t>
         </is>
       </c>
     </row>
@@ -17009,152 +17009,152 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>11/32 (34.4%)</t>
+          <t>7/32 (21.9%)</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
+          <t>2/32 (6.2%)</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>16/32 (50.0%)</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>6/32 (18.8%)</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>16/32 (50.0%)</t>
+        </is>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>6/32 (18.8%)</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>5/32 (15.6%)</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="N115" t="inlineStr">
+        <is>
           <t>14/32 (43.8%)</t>
         </is>
       </c>
-      <c r="D115" t="inlineStr">
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>8/32 (25.0%)</t>
+        </is>
+      </c>
+      <c r="P115" t="inlineStr">
+        <is>
+          <t>6/32 (18.8%)</t>
+        </is>
+      </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>8/32 (25.0%)</t>
+        </is>
+      </c>
+      <c r="R115" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="S115" t="inlineStr">
+        <is>
+          <t>2/32 (6.2%)</t>
+        </is>
+      </c>
+      <c r="T115" t="inlineStr">
+        <is>
+          <t>13/32 (40.6%)</t>
+        </is>
+      </c>
+      <c r="U115" t="inlineStr">
+        <is>
+          <t>6/32 (18.8%)</t>
+        </is>
+      </c>
+      <c r="V115" t="inlineStr">
+        <is>
+          <t>6/32 (18.8%)</t>
+        </is>
+      </c>
+      <c r="W115" t="inlineStr">
+        <is>
+          <t>16/32 (50.0%)</t>
+        </is>
+      </c>
+      <c r="X115" t="inlineStr">
+        <is>
+          <t>8/32 (25.0%)</t>
+        </is>
+      </c>
+      <c r="Y115" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="Z115" t="inlineStr">
+        <is>
+          <t>5/32 (15.6%)</t>
+        </is>
+      </c>
+      <c r="AA115" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="AB115" t="inlineStr">
+        <is>
+          <t>8/32 (25.0%)</t>
+        </is>
+      </c>
+      <c r="AC115" t="inlineStr">
+        <is>
+          <t>12/32 (37.5%)</t>
+        </is>
+      </c>
+      <c r="AD115" t="inlineStr">
+        <is>
+          <t>6/32 (18.8%)</t>
+        </is>
+      </c>
+      <c r="AE115" t="inlineStr">
         <is>
           <t>7/32 (21.9%)</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>12/32 (37.5%)</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>15/32 (46.9%)</t>
-        </is>
-      </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>1/32 (3.1%)</t>
-        </is>
-      </c>
-      <c r="H115" t="inlineStr">
-        <is>
-          <t>2/32 (6.2%)</t>
-        </is>
-      </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>1/32 (3.1%)</t>
-        </is>
-      </c>
-      <c r="J115" t="inlineStr">
-        <is>
-          <t>6/32 (18.8%)</t>
-        </is>
-      </c>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>2/32 (6.2%)</t>
-        </is>
-      </c>
-      <c r="L115" t="inlineStr">
-        <is>
-          <t>8/32 (25.0%)</t>
-        </is>
-      </c>
-      <c r="M115" t="inlineStr">
-        <is>
-          <t>5/32 (15.6%)</t>
-        </is>
-      </c>
-      <c r="N115" t="inlineStr">
-        <is>
-          <t>2/32 (6.2%)</t>
-        </is>
-      </c>
-      <c r="O115" t="inlineStr">
-        <is>
-          <t>9/32 (28.1%)</t>
-        </is>
-      </c>
-      <c r="P115" t="inlineStr">
-        <is>
-          <t>7/32 (21.9%)</t>
-        </is>
-      </c>
-      <c r="Q115" t="inlineStr">
-        <is>
-          <t>1/32 (3.1%)</t>
-        </is>
-      </c>
-      <c r="R115" t="inlineStr">
-        <is>
-          <t>5/32 (15.6%)</t>
-        </is>
-      </c>
-      <c r="S115" t="inlineStr">
-        <is>
-          <t>11/32 (34.4%)</t>
-        </is>
-      </c>
-      <c r="T115" t="inlineStr">
-        <is>
-          <t>8/32 (25.0%)</t>
-        </is>
-      </c>
-      <c r="U115" t="inlineStr">
-        <is>
-          <t>1/32 (3.1%)</t>
-        </is>
-      </c>
-      <c r="V115" t="inlineStr">
-        <is>
-          <t>10/32 (31.2%)</t>
-        </is>
-      </c>
-      <c r="W115" t="inlineStr">
-        <is>
-          <t>3/32 (9.4%)</t>
-        </is>
-      </c>
-      <c r="X115" t="inlineStr">
-        <is>
-          <t>8/32 (25.0%)</t>
-        </is>
-      </c>
-      <c r="Y115" t="inlineStr">
-        <is>
-          <t>1/32 (3.1%)</t>
-        </is>
-      </c>
-      <c r="Z115" t="inlineStr">
-        <is>
-          <t>17/32 (53.1%)</t>
-        </is>
-      </c>
-      <c r="AA115" t="inlineStr">
-        <is>
-          <t>7/32 (21.9%)</t>
-        </is>
-      </c>
-      <c r="AB115" t="inlineStr">
-        <is>
-          <t>9/32 (28.1%)</t>
-        </is>
-      </c>
-      <c r="AC115" t="inlineStr">
-        <is>
-          <t>7/32 (21.9%)</t>
-        </is>
-      </c>
-      <c r="AD115" t="inlineStr">
-        <is>
-          <t>17/32 (53.1%)</t>
-        </is>
-      </c>
-      <c r="AE115" t="inlineStr">
-        <is>
-          <t>8/32 (25.0%)</t>
         </is>
       </c>
     </row>
@@ -17166,152 +17166,152 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>0.1859</t>
+          <t>0.0181</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>0.4440</t>
+          <t>0.0020</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>0.0767</t>
+          <t>0.5326</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>0.1321</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>0.6210</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>0.0002</t>
+          <t>0.0059</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>0.0008</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.2684</t>
         </is>
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>0.1279</t>
+          <t>0.0064</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
         <is>
-          <t>0.0002</t>
+          <t>0.0032</t>
         </is>
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>0.0122</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="M116" t="inlineStr">
         <is>
-          <t>0.0056</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>0.0011</t>
+          <t>0.1728</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
         <is>
-          <t>0.2458</t>
+          <t>0.0474</t>
         </is>
       </c>
       <c r="P116" t="inlineStr">
         <is>
-          <t>0.1753</t>
+          <t>0.0347</t>
         </is>
       </c>
       <c r="Q116" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.0553</t>
         </is>
       </c>
       <c r="R116" t="inlineStr">
         <is>
-          <t>0.0023</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="S116" t="inlineStr">
         <is>
-          <t>0.1714</t>
+          <t>0.0010</t>
         </is>
       </c>
       <c r="T116" t="inlineStr">
         <is>
-          <t>0.3120</t>
+          <t>0.0304</t>
         </is>
       </c>
       <c r="U116" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.1555</t>
         </is>
       </c>
       <c r="V116" t="inlineStr">
         <is>
-          <t>0.0462</t>
+          <t>0.0278</t>
         </is>
       </c>
       <c r="W116" t="inlineStr">
         <is>
-          <t>0.0048</t>
+          <t>0.0463</t>
         </is>
       </c>
       <c r="X116" t="inlineStr">
         <is>
-          <t>0.3298</t>
+          <t>0.0491</t>
         </is>
       </c>
       <c r="Y116" t="inlineStr">
         <is>
-          <t>0.0001</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="Z116" t="inlineStr">
         <is>
-          <t>0.5495</t>
+          <t>0.0072</t>
         </is>
       </c>
       <c r="AA116" t="inlineStr">
         <is>
-          <t>0.0929</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="AB116" t="inlineStr">
         <is>
-          <t>0.1332</t>
+          <t>0.2834</t>
         </is>
       </c>
       <c r="AC116" t="inlineStr">
         <is>
-          <t>0.3511</t>
+          <t>0.1405</t>
         </is>
       </c>
       <c r="AD116" t="inlineStr">
         <is>
-          <t>0.2125</t>
+          <t>0.0369</t>
         </is>
       </c>
       <c r="AE116" t="inlineStr">
         <is>
-          <t>0.1089</t>
+          <t>0.0225</t>
         </is>
       </c>
     </row>
@@ -17323,152 +17323,152 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
+          <t>13/21 (61.9%)</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>5/21 (23.8%)</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>6/21 (28.6%)</t>
+        </is>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>2/21 (9.5%)</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>12/21 (57.1%)</t>
+        </is>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>4/21 (19.0%)</t>
+        </is>
+      </c>
+      <c r="P117" t="inlineStr">
+        <is>
+          <t>2/21 (9.5%)</t>
+        </is>
+      </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>3/21 (14.3%)</t>
+        </is>
+      </c>
+      <c r="R117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="S117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="T117" t="inlineStr">
+        <is>
+          <t>7/21 (33.3%)</t>
+        </is>
+      </c>
+      <c r="U117" t="inlineStr">
+        <is>
+          <t>6/21 (28.6%)</t>
+        </is>
+      </c>
+      <c r="V117" t="inlineStr">
+        <is>
+          <t>4/21 (19.0%)</t>
+        </is>
+      </c>
+      <c r="W117" t="inlineStr">
+        <is>
+          <t>13/21 (61.9%)</t>
+        </is>
+      </c>
+      <c r="X117" t="inlineStr">
+        <is>
+          <t>4/21 (19.0%)</t>
+        </is>
+      </c>
+      <c r="Y117" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="Z117" t="inlineStr">
+        <is>
+          <t>11/21 (52.4%)</t>
+        </is>
+      </c>
+      <c r="AA117" t="inlineStr">
+        <is>
+          <t>3/21 (14.3%)</t>
+        </is>
+      </c>
+      <c r="AB117" t="inlineStr">
+        <is>
+          <t>11/21 (52.4%)</t>
+        </is>
+      </c>
+      <c r="AC117" t="inlineStr">
+        <is>
+          <t>13/21 (61.9%)</t>
+        </is>
+      </c>
+      <c r="AD117" t="inlineStr">
+        <is>
           <t>9/21 (42.9%)</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>10/21 (47.6%)</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>6/21 (28.6%)</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>10/21 (47.6%)</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
+      <c r="AE117" t="inlineStr">
         <is>
           <t>9/21 (42.9%)</t>
-        </is>
-      </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="H117" t="inlineStr">
-        <is>
-          <t>1/21 (4.8%)</t>
-        </is>
-      </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="J117" t="inlineStr">
-        <is>
-          <t>6/21 (28.6%)</t>
-        </is>
-      </c>
-      <c r="K117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="L117" t="inlineStr">
-        <is>
-          <t>5/21 (23.8%)</t>
-        </is>
-      </c>
-      <c r="M117" t="inlineStr">
-        <is>
-          <t>4/21 (19.0%)</t>
-        </is>
-      </c>
-      <c r="N117" t="inlineStr">
-        <is>
-          <t>1/21 (4.8%)</t>
-        </is>
-      </c>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>7/21 (33.3%)</t>
-        </is>
-      </c>
-      <c r="P117" t="inlineStr">
-        <is>
-          <t>5/21 (23.8%)</t>
-        </is>
-      </c>
-      <c r="Q117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="R117" t="inlineStr">
-        <is>
-          <t>1/21 (4.8%)</t>
-        </is>
-      </c>
-      <c r="S117" t="inlineStr">
-        <is>
-          <t>11/21 (52.4%)</t>
-        </is>
-      </c>
-      <c r="T117" t="inlineStr">
-        <is>
-          <t>6/21 (28.6%)</t>
-        </is>
-      </c>
-      <c r="U117" t="inlineStr">
-        <is>
-          <t>0/21 (0.0%)</t>
-        </is>
-      </c>
-      <c r="V117" t="inlineStr">
-        <is>
-          <t>9/21 (42.9%)</t>
-        </is>
-      </c>
-      <c r="W117" t="inlineStr">
-        <is>
-          <t>3/21 (14.3%)</t>
-        </is>
-      </c>
-      <c r="X117" t="inlineStr">
-        <is>
-          <t>7/21 (33.3%)</t>
-        </is>
-      </c>
-      <c r="Y117" t="inlineStr">
-        <is>
-          <t>1/21 (4.8%)</t>
-        </is>
-      </c>
-      <c r="Z117" t="inlineStr">
-        <is>
-          <t>13/21 (61.9%)</t>
-        </is>
-      </c>
-      <c r="AA117" t="inlineStr">
-        <is>
-          <t>6/21 (28.6%)</t>
-        </is>
-      </c>
-      <c r="AB117" t="inlineStr">
-        <is>
-          <t>5/21 (23.8%)</t>
-        </is>
-      </c>
-      <c r="AC117" t="inlineStr">
-        <is>
-          <t>6/21 (28.6%)</t>
-        </is>
-      </c>
-      <c r="AD117" t="inlineStr">
-        <is>
-          <t>13/21 (61.9%)</t>
-        </is>
-      </c>
-      <c r="AE117" t="inlineStr">
-        <is>
-          <t>5/21 (23.8%)</t>
         </is>
       </c>
     </row>
@@ -17480,152 +17480,152 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>0.4792</t>
+          <t>0.0518</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>0.1133</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>0.1109</t>
+          <t>0.0317</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>0.0889</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>0.5297</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0010</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>0.0007</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.1097</t>
         </is>
       </c>
       <c r="J118" t="inlineStr">
         <is>
+          <t>0.0009</t>
+        </is>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>0.0001</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>0.0762</t>
+        </is>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>0.0294</t>
+        </is>
+      </c>
+      <c r="P118" t="inlineStr">
+        <is>
+          <t>0.0848</t>
+        </is>
+      </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>0.0457</t>
+        </is>
+      </c>
+      <c r="R118" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="S118" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="T118" t="inlineStr">
+        <is>
           <t>0.0131</t>
         </is>
       </c>
-      <c r="K118" t="inlineStr">
-        <is>
-          <t>0.0000</t>
-        </is>
-      </c>
-      <c r="L118" t="inlineStr">
-        <is>
-          <t>0.0066</t>
-        </is>
-      </c>
-      <c r="M118" t="inlineStr">
-        <is>
-          <t>0.0032</t>
-        </is>
-      </c>
-      <c r="N118" t="inlineStr">
-        <is>
-          <t>0.0002</t>
-        </is>
-      </c>
-      <c r="O118" t="inlineStr">
-        <is>
-          <t>0.0386</t>
-        </is>
-      </c>
-      <c r="P118" t="inlineStr">
-        <is>
-          <t>0.0903</t>
-        </is>
-      </c>
-      <c r="Q118" t="inlineStr">
-        <is>
-          <t>0.0000</t>
-        </is>
-      </c>
-      <c r="R118" t="inlineStr">
-        <is>
-          <t>0.0005</t>
-        </is>
-      </c>
-      <c r="S118" t="inlineStr">
-        <is>
-          <t>0.0228</t>
-        </is>
-      </c>
-      <c r="T118" t="inlineStr">
-        <is>
-          <t>0.0383</t>
-        </is>
-      </c>
       <c r="U118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>0.0098</t>
         </is>
       </c>
       <c r="V118" t="inlineStr">
         <is>
-          <t>0.0779</t>
+          <t>0.0418</t>
         </is>
       </c>
       <c r="W118" t="inlineStr">
         <is>
-          <t>0.0127</t>
+          <t>0.1689</t>
         </is>
       </c>
       <c r="X118" t="inlineStr">
         <is>
-          <t>1.1824</t>
+          <t>0.0073</t>
         </is>
       </c>
       <c r="Y118" t="inlineStr">
         <is>
-          <t>0.0002</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="Z118" t="inlineStr">
         <is>
-          <t>0.5050</t>
+          <t>0.1035</t>
         </is>
       </c>
       <c r="AA118" t="inlineStr">
         <is>
-          <t>0.1086</t>
+          <t>0.0019</t>
         </is>
       </c>
       <c r="AB118" t="inlineStr">
         <is>
-          <t>0.2151</t>
+          <t>1.5101</t>
         </is>
       </c>
       <c r="AC118" t="inlineStr">
         <is>
-          <t>0.6372</t>
+          <t>1.1856</t>
         </is>
       </c>
       <c r="AD118" t="inlineStr">
         <is>
-          <t>0.2058</t>
+          <t>0.4448</t>
         </is>
       </c>
       <c r="AE118" t="inlineStr">
         <is>
-          <t>0.1810</t>
+          <t>0.2507</t>
         </is>
       </c>
     </row>

</xml_diff>